<commit_message>
ADO.NET for MsSQL bench. Bench rerun.
Manual SQL with hand materialization for MS SQL Server

TODO: Bulk update for mssql on standard and complex
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -15,13 +15,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="29">
   <si>
     <t>Simple</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Npgsql</t>
   </si>
   <si>
-    <t>Revenj Postgres</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -112,6 +109,12 @@
       </rPr>
       <t>Unlicensed version. Please register @ templater.info</t>
     </r>
+  </si>
+  <si>
+    <t>Revenj</t>
+  </si>
+  <si>
+    <t>Entity Framework</t>
   </si>
 </sst>
 </file>
@@ -215,78 +218,62 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="4"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="5"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="6"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="7"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="8"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="9"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="10"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="11"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -306,7 +293,47 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="13"/>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent2"/>
@@ -314,6 +341,26 @@
           <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent2">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
                 <a:shade val="50000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -409,31 +456,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1127</c:v>
+                  <c:v>1160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1613</c:v>
+                  <c:v>1612</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5224</c:v>
+                  <c:v>4933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5512</c:v>
+                  <c:v>5399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1103</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2652</c:v>
+                  <c:v>2636</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>773</c:v>
+                  <c:v>805</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>497</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>739</c:v>
+                  <c:v>686</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -448,7 +495,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Revenj Postgres</c:v>
+                  <c:v>Revenj</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -522,31 +569,144 @@
                   <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5023</c:v>
+                  <c:v>4978</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4986</c:v>
+                  <c:v>4914</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1983</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>417</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1487</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1081</c:v>
+                  <c:v>1064</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>728</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>469</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>694</c:v>
+                  <c:v>687</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Simple!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entity Framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Simple!$A$3:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Simple!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3119</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2788</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2721</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,11 +721,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101673216"/>
-        <c:axId val="138088448"/>
+        <c:axId val="84563072"/>
+        <c:axId val="84564608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101673216"/>
+        <c:axId val="84563072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +734,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138088448"/>
+        <c:crossAx val="84564608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -582,7 +742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138088448"/>
+        <c:axId val="84564608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +773,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101673216"/>
+        <c:crossAx val="84563072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -910,6 +1070,32 @@
         <c:idx val="36"/>
         <c:spPr>
           <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="37"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="38"/>
+        <c:spPr>
+          <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
@@ -927,7 +1113,76 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="37"/>
+        <c:idx val="39"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="40"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="41"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="42"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="43"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="44"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent2"/>
@@ -947,7 +1202,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="38"/>
+        <c:idx val="45"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent6"/>
@@ -955,6 +1210,32 @@
           <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent6">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="46"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="47"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
                 <a:shade val="50000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -1116,31 +1397,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1294</c:v>
+                  <c:v>1306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1477</c:v>
+                  <c:v>1490</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1120</c:v>
+                  <c:v>1256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1441</c:v>
+                  <c:v>1480</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3930</c:v>
+                  <c:v>3908</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3133</c:v>
+                  <c:v>3158</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3793</c:v>
+                  <c:v>3859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2827</c:v>
+                  <c:v>2831</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2195</c:v>
+                  <c:v>2205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,7 +1436,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Revenj Postgres - NoSQL</c:v>
+                  <c:v>Revenj - NoSQL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1238,13 +1519,13 @@
                   <c:v>991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>950</c:v>
+                  <c:v>995</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>769</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1316</c:v>
+                  <c:v>1325</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1473</c:v>
@@ -1253,7 +1534,7 @@
                   <c:v>957</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>941</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,7 +1549,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Revenj Postgres - Relational</c:v>
+                  <c:v>Revenj - Relational</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1372,6 +1653,185 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Standard!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entity Framework - NoSQL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Standard!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Standard!$F$4:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Standard!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entity Framework - Relational</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Standard!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Standard!$G$4:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2454</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12269</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2686</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7181</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1381,11 +1841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147514112"/>
-        <c:axId val="147515648"/>
+        <c:axId val="84792064"/>
+        <c:axId val="84793600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147514112"/>
+        <c:axId val="84792064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1854,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147515648"/>
+        <c:crossAx val="84793600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1402,7 +1862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147515648"/>
+        <c:axId val="84793600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1893,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147514112"/>
+        <c:crossAx val="84792064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1862,6 +2322,32 @@
         <c:idx val="58"/>
         <c:spPr>
           <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="59"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="60"/>
+        <c:spPr>
+          <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
@@ -1879,7 +2365,73 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="59"/>
+        <c:idx val="61"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="62"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="63"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="64"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="65"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent2"/>
@@ -1899,7 +2451,7 @@
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="60"/>
+        <c:idx val="66"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent6"/>
@@ -1907,6 +2459,32 @@
           <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent6">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="67"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="68"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
                 <a:shade val="50000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -2068,31 +2646,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>36206</c:v>
+                  <c:v>35410</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44207</c:v>
+                  <c:v>46748</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9791</c:v>
+                  <c:v>12673</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12093</c:v>
+                  <c:v>13186</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72376</c:v>
+                  <c:v>70935</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47318</c:v>
+                  <c:v>51564</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>101261</c:v>
+                  <c:v>106610</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>86261</c:v>
+                  <c:v>113597</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19787</c:v>
+                  <c:v>19171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,7 +2685,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Revenj Postgres - NoSQL</c:v>
+                  <c:v>Revenj - NoSQL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2184,7 +2762,7 @@
                   <c:v>605</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>703</c:v>
+                  <c:v>652</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17217</c:v>
@@ -2205,7 +2783,7 @@
                   <c:v>31446</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11758</c:v>
+                  <c:v>10649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2220,7 +2798,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Revenj Postgres - Relational</c:v>
+                  <c:v>Revenj - Relational</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2288,7 +2866,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7110</c:v>
+                  <c:v>7006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>695</c:v>
@@ -2319,6 +2897,185 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>15981</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Complex!$F$1:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entity Framework - NoSQL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Complex!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Complex!$F$4:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Complex!$G$1:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entity Framework - Relational</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Complex!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Complex!$G$4:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>93677</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36186</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5838</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>298963</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>281792</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>202582</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650882</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>563322</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>141763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2333,11 +3090,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148728832"/>
-        <c:axId val="148755200"/>
+        <c:axId val="85275008"/>
+        <c:axId val="85276544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148728832"/>
+        <c:axId val="85275008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2346,7 +3103,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148755200"/>
+        <c:crossAx val="85276544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2354,7 +3111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148755200"/>
+        <c:axId val="85276544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2385,7 +3142,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148728832"/>
+        <c:crossAx val="85275008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2459,14 +3216,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>142873</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2500,10 +3257,10 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>981074</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2528,7 +3285,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42071.870035763888" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="22">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42081.82422962963" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="33">
   <cacheSource type="worksheet">
     <worksheetSource name="Table3"/>
   </cacheSource>
@@ -2546,32 +3303,36 @@
         <s v="Find many (x2.000)"/>
         <s v="Find one (x5.000)"/>
         <s v="Report (x1.000)"/>
+        <s v="Find many (x10.000)" u="1"/>
         <s v="Search subset (x5.000)" u="1"/>
-        <s v="Find many (x10.000)" u="1"/>
+        <s v="Find one (x10.000)" u="1"/>
         <s v="Query all (x1.000)" u="1"/>
-        <s v="Find one (x10.000)" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Simple" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="123" maxValue="5512"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="123" maxValue="17136"/>
     </cacheField>
     <cacheField name="Standard objects" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="52" maxValue="1473"/>
     </cacheField>
     <cacheField name="Standard relations" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="102" maxValue="3930"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="102" maxValue="21160"/>
     </cacheField>
     <cacheField name="Complex objects" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="605" maxValue="37827"/>
     </cacheField>
     <cacheField name="Complex relations" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="695" maxValue="101261"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="695" maxValue="650882"/>
     </cacheField>
     <cacheField name="Target" numFmtId="0">
-      <sharedItems count="3">
+      <sharedItems count="7">
         <s v="Npgsql"/>
-        <s v="Revenj Postgres"/>
+        <s v="Revenj"/>
+        <s v="Entity Framework"/>
+        <s v="Revenj Postgres" u="1"/>
+        <s v="MsSql ADO.NET" u="1"/>
         <s v="[[description]]" u="1"/>
+        <s v="EF Postgres" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2584,59 +3345,59 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="22">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="33">
   <r>
     <x v="0"/>
-    <n v="1127"/>
+    <n v="1160"/>
     <m/>
-    <n v="1294"/>
+    <n v="1306"/>
     <m/>
-    <n v="36206"/>
+    <n v="35410"/>
     <x v="0"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="1613"/>
+    <n v="1612"/>
     <m/>
-    <n v="1477"/>
+    <n v="1490"/>
     <m/>
-    <n v="44207"/>
+    <n v="46748"/>
     <x v="0"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="5224"/>
+    <n v="4933"/>
     <m/>
-    <n v="1120"/>
+    <n v="1256"/>
     <m/>
-    <n v="9791"/>
+    <n v="12673"/>
     <x v="0"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="5512"/>
+    <n v="5399"/>
     <m/>
-    <n v="1441"/>
+    <n v="1480"/>
     <m/>
-    <n v="12093"/>
+    <n v="13186"/>
     <x v="0"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="2652"/>
+    <n v="2636"/>
     <m/>
-    <n v="3133"/>
+    <n v="3158"/>
     <m/>
-    <n v="47318"/>
+    <n v="51564"/>
     <x v="0"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="773"/>
+    <n v="805"/>
     <m/>
-    <n v="3793"/>
+    <n v="3859"/>
     <m/>
-    <n v="101261"/>
+    <n v="106610"/>
     <x v="0"/>
   </r>
   <r>
@@ -2659,29 +3420,29 @@
   </r>
   <r>
     <x v="8"/>
-    <n v="497"/>
+    <n v="506"/>
     <m/>
-    <n v="2827"/>
+    <n v="2831"/>
     <m/>
-    <n v="86261"/>
+    <n v="113597"/>
     <x v="0"/>
   </r>
   <r>
     <x v="9"/>
-    <n v="739"/>
+    <n v="686"/>
     <m/>
-    <n v="2195"/>
+    <n v="2205"/>
     <m/>
-    <n v="19787"/>
+    <n v="19171"/>
     <x v="0"/>
   </r>
   <r>
     <x v="10"/>
-    <n v="1103"/>
+    <n v="1080"/>
     <m/>
-    <n v="3930"/>
+    <n v="3908"/>
     <m/>
-    <n v="72376"/>
+    <n v="70935"/>
     <x v="0"/>
   </r>
   <r>
@@ -2690,7 +3451,7 @@
     <n v="52"/>
     <n v="213"/>
     <n v="2193"/>
-    <n v="7110"/>
+    <n v="7006"/>
     <x v="1"/>
   </r>
   <r>
@@ -2704,7 +3465,7 @@
   </r>
   <r>
     <x v="2"/>
-    <n v="5023"/>
+    <n v="4978"/>
     <n v="503"/>
     <n v="1038"/>
     <n v="605"/>
@@ -2713,10 +3474,10 @@
   </r>
   <r>
     <x v="3"/>
-    <n v="4986"/>
+    <n v="4914"/>
     <n v="422"/>
     <n v="849"/>
-    <n v="703"/>
+    <n v="652"/>
     <n v="3625"/>
     <x v="1"/>
   </r>
@@ -2731,7 +3492,7 @@
   </r>
   <r>
     <x v="5"/>
-    <n v="728"/>
+    <n v="712"/>
     <n v="1473"/>
     <n v="2597"/>
     <n v="37827"/>
@@ -2749,8 +3510,8 @@
   </r>
   <r>
     <x v="7"/>
-    <n v="1081"/>
-    <n v="1316"/>
+    <n v="1064"/>
+    <n v="1325"/>
     <n v="1693"/>
     <n v="12877"/>
     <n v="19017"/>
@@ -2758,7 +3519,7 @@
   </r>
   <r>
     <x v="8"/>
-    <n v="469"/>
+    <n v="497"/>
     <n v="957"/>
     <n v="1723"/>
     <n v="31446"/>
@@ -2767,42 +3528,141 @@
   </r>
   <r>
     <x v="9"/>
-    <n v="694"/>
-    <n v="941"/>
+    <n v="687"/>
+    <n v="961"/>
     <n v="1751"/>
-    <n v="11758"/>
+    <n v="10649"/>
     <n v="15981"/>
     <x v="1"/>
   </r>
   <r>
     <x v="10"/>
-    <n v="417"/>
-    <n v="950"/>
+    <n v="410"/>
+    <n v="995"/>
     <n v="1708"/>
     <n v="32380"/>
     <n v="44228"/>
     <x v="1"/>
   </r>
+  <r>
+    <x v="0"/>
+    <n v="3119"/>
+    <m/>
+    <n v="2100"/>
+    <m/>
+    <n v="93677"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2788"/>
+    <m/>
+    <n v="836"/>
+    <m/>
+    <n v="36186"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="12331"/>
+    <m/>
+    <n v="2454"/>
+    <m/>
+    <n v="20147"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="13345"/>
+    <m/>
+    <n v="1588"/>
+    <m/>
+    <n v="5838"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2288"/>
+    <m/>
+    <n v="12269"/>
+    <m/>
+    <n v="281792"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="2721"/>
+    <m/>
+    <n v="7181"/>
+    <m/>
+    <n v="650882"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="2305"/>
+    <m/>
+    <n v="12315"/>
+    <m/>
+    <n v="298963"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="1187"/>
+    <m/>
+    <n v="2686"/>
+    <m/>
+    <n v="202582"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="4968"/>
+    <m/>
+    <n v="16006"/>
+    <m/>
+    <n v="563322"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="9384"/>
+    <m/>
+    <n v="15297"/>
+    <m/>
+    <n v="141763"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="17136"/>
+    <m/>
+    <n v="21160"/>
+    <m/>
+    <n v="23924"/>
+    <x v="2"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
       <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="12"/>
-        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="13"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
-        <item m="1" x="11"/>
+        <item m="1" x="12"/>
         <item x="7"/>
         <item x="5"/>
         <item x="8"/>
@@ -2816,10 +3676,14 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item m="1" x="2"/>
+      <items count="8">
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
         <item x="0"/>
+        <item m="1" x="3"/>
+        <item m="1" x="6"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2868,12 +3732,15 @@
   <colFields count="1">
     <field x="6"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -2882,7 +3749,7 @@
   <dataFields count="1">
     <dataField name="Relational" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="14">
+  <chartFormats count="18">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3014,6 +3881,54 @@
           </reference>
           <reference field="6" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -3029,22 +3944,22 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A1:G15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A1:I15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
       <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="12"/>
-        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="13"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
-        <item m="1" x="11"/>
+        <item m="1" x="12"/>
         <item x="7"/>
         <item x="5"/>
         <item x="8"/>
@@ -3058,10 +3973,14 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item m="1" x="2"/>
+      <items count="8">
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
         <item x="0"/>
+        <item m="1" x="3"/>
+        <item m="1" x="6"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3111,16 +4030,23 @@
     <field x="6"/>
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="8">
     <i>
-      <x v="1"/>
+      <x v="2"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
       <x/>
     </i>
     <i r="1" i="1">
@@ -3137,7 +4063,7 @@
     <dataField name="NoSQL" fld="2" baseField="0" baseItem="0"/>
     <dataField name="Relational" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="28">
+  <chartFormats count="37">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3437,6 +4363,117 @@
           </reference>
           <reference field="6" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="39" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="40" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="41" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="42" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="43">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="44" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="45" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="46" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="47" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -3452,22 +4489,22 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A1:G15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A1:I15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
       <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="12"/>
-        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="13"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
-        <item m="1" x="11"/>
+        <item m="1" x="12"/>
         <item x="7"/>
         <item x="5"/>
         <item x="8"/>
@@ -3481,10 +4518,14 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item m="1" x="2"/>
+      <items count="8">
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
         <item x="0"/>
+        <item m="1" x="3"/>
+        <item m="1" x="6"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3534,16 +4575,23 @@
     <field x="6"/>
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="8">
     <i>
-      <x v="1"/>
+      <x v="2"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
       <x/>
     </i>
     <i r="1" i="1">
@@ -3560,7 +4608,7 @@
     <dataField name="NoSQL" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Relational" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="28">
+  <chartFormats count="36">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3827,6 +4875,102 @@
           </reference>
           <reference field="6" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="61" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="62" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="63" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="64" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="65" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="66" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="67" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="68" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -3842,8 +4986,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:G23" totalsRowShown="0">
-  <autoFilter ref="A1:G23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:G34" totalsRowShown="0">
+  <autoFilter ref="A1:G34"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Bench type"/>
     <tableColumn id="2" name="Simple"/>
@@ -4152,7 +5296,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4162,11 +5306,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4207,13 +5349,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1127</v>
+        <v>1160</v>
       </c>
       <c r="D2">
-        <v>1294</v>
+        <v>1306</v>
       </c>
       <c r="F2">
-        <v>36206</v>
+        <v>35410</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
@@ -4224,13 +5366,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D3">
-        <v>1477</v>
+        <v>1490</v>
       </c>
       <c r="F3">
-        <v>44207</v>
+        <v>46748</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
@@ -4241,13 +5383,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>5224</v>
+        <v>4933</v>
       </c>
       <c r="D4">
-        <v>1120</v>
+        <v>1256</v>
       </c>
       <c r="F4">
-        <v>9791</v>
+        <v>12673</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -4258,13 +5400,13 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>5512</v>
+        <v>5399</v>
       </c>
       <c r="D5">
-        <v>1441</v>
+        <v>1480</v>
       </c>
       <c r="F5">
-        <v>12093</v>
+        <v>13186</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -4275,13 +5417,13 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2652</v>
+        <v>2636</v>
       </c>
       <c r="D6">
-        <v>3133</v>
+        <v>3158</v>
       </c>
       <c r="F6">
-        <v>47318</v>
+        <v>51564</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
@@ -4292,13 +5434,13 @@
         <v>22</v>
       </c>
       <c r="B7">
-        <v>773</v>
+        <v>805</v>
       </c>
       <c r="D7">
-        <v>3793</v>
+        <v>3859</v>
       </c>
       <c r="F7">
-        <v>101261</v>
+        <v>106610</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
@@ -4325,13 +5467,13 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="D10">
-        <v>2827</v>
+        <v>2831</v>
       </c>
       <c r="F10">
-        <v>86261</v>
+        <v>113597</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -4342,13 +5484,13 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>739</v>
+        <v>686</v>
       </c>
       <c r="D11">
-        <v>2195</v>
+        <v>2205</v>
       </c>
       <c r="F11">
-        <v>19787</v>
+        <v>19171</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
@@ -4359,13 +5501,13 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1103</v>
+        <v>1080</v>
       </c>
       <c r="D12">
-        <v>3930</v>
+        <v>3908</v>
       </c>
       <c r="F12">
-        <v>72376</v>
+        <v>70935</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -4388,10 +5530,10 @@
         <v>2193</v>
       </c>
       <c r="F13">
-        <v>7110</v>
+        <v>7006</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4414,7 +5556,7 @@
         <v>695</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4422,7 +5564,7 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>5023</v>
+        <v>4978</v>
       </c>
       <c r="C15">
         <v>503</v>
@@ -4437,7 +5579,7 @@
         <v>3213</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4445,7 +5587,7 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>4986</v>
+        <v>4914</v>
       </c>
       <c r="C16">
         <v>422</v>
@@ -4454,13 +5596,13 @@
         <v>849</v>
       </c>
       <c r="E16">
-        <v>703</v>
+        <v>652</v>
       </c>
       <c r="F16">
         <v>3625</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4483,7 +5625,7 @@
         <v>25812</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4491,7 +5633,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>728</v>
+        <v>712</v>
       </c>
       <c r="C18">
         <v>1473</v>
@@ -4506,7 +5648,7 @@
         <v>58402</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4529,7 +5671,7 @@
         <v>26094</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4537,10 +5679,10 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>1081</v>
+        <v>1064</v>
       </c>
       <c r="C20">
-        <v>1316</v>
+        <v>1325</v>
       </c>
       <c r="D20">
         <v>1693</v>
@@ -4552,7 +5694,7 @@
         <v>19017</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4560,7 +5702,7 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>469</v>
+        <v>497</v>
       </c>
       <c r="C21">
         <v>957</v>
@@ -4575,7 +5717,7 @@
         <v>48448</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4583,22 +5725,22 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="C22">
-        <v>941</v>
+        <v>961</v>
       </c>
       <c r="D22">
         <v>1751</v>
       </c>
       <c r="E22">
-        <v>11758</v>
+        <v>10649</v>
       </c>
       <c r="F22">
         <v>15981</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4606,10 +5748,10 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C23">
-        <v>950</v>
+        <v>995</v>
       </c>
       <c r="D23">
         <v>1708</v>
@@ -4621,7 +5763,194 @@
         <v>44228</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>3119</v>
+      </c>
+      <c r="D24">
+        <v>2100</v>
+      </c>
+      <c r="F24">
+        <v>93677</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>2788</v>
+      </c>
+      <c r="D25">
+        <v>836</v>
+      </c>
+      <c r="F25">
+        <v>36186</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>12331</v>
+      </c>
+      <c r="D26">
+        <v>2454</v>
+      </c>
+      <c r="F26">
+        <v>20147</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>13345</v>
+      </c>
+      <c r="D27">
+        <v>1588</v>
+      </c>
+      <c r="F27">
+        <v>5838</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>2288</v>
+      </c>
+      <c r="D28">
+        <v>12269</v>
+      </c>
+      <c r="F28">
+        <v>281792</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>2721</v>
+      </c>
+      <c r="D29">
+        <v>7181</v>
+      </c>
+      <c r="F29">
+        <v>650882</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>2305</v>
+      </c>
+      <c r="D30">
+        <v>12315</v>
+      </c>
+      <c r="F30">
+        <v>298963</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>1187</v>
+      </c>
+      <c r="D31">
+        <v>2686</v>
+      </c>
+      <c r="F31">
+        <v>202582</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32">
+        <v>4968</v>
+      </c>
+      <c r="D32">
+        <v>16006</v>
+      </c>
+      <c r="F32">
+        <v>563322</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>9384</v>
+      </c>
+      <c r="D33">
+        <v>15297</v>
+      </c>
+      <c r="F33">
+        <v>141763</v>
+      </c>
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>17136</v>
+      </c>
+      <c r="D34">
+        <v>21160</v>
+      </c>
+      <c r="F34">
+        <v>23924</v>
+      </c>
+      <c r="G34" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -4635,20 +5964,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -4669,7 +5997,7 @@
     <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4677,7 +6005,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -4685,69 +6013,84 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>1127</v>
+        <v>1160</v>
       </c>
       <c r="C3" s="3">
         <v>123</v>
       </c>
       <c r="D3" s="3">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3119</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C4" s="3">
         <v>224</v>
       </c>
       <c r="D4" s="3">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2788</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3">
-        <v>5224</v>
+        <v>4933</v>
       </c>
       <c r="C5" s="3">
-        <v>5023</v>
+        <v>4978</v>
       </c>
       <c r="D5" s="3">
-        <v>10247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12331</v>
+      </c>
+      <c r="E5" s="3">
+        <v>22242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>5512</v>
+        <v>5399</v>
       </c>
       <c r="C6" s="3">
-        <v>4986</v>
+        <v>4914</v>
       </c>
       <c r="D6" s="3">
-        <v>10498</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13345</v>
+      </c>
+      <c r="E6" s="3">
+        <v>23658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4756,103 +6099,127 @@
         <v>1983</v>
       </c>
       <c r="D7" s="3">
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2305</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3">
-        <v>1103</v>
+        <v>1080</v>
       </c>
       <c r="C8" s="3">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="D8" s="3">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17136</v>
+      </c>
+      <c r="E8" s="3">
+        <v>18626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>2652</v>
+        <v>2636</v>
       </c>
       <c r="C9" s="3">
         <v>1487</v>
       </c>
       <c r="D9" s="3">
-        <v>4139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2288</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
-        <v>1081</v>
+        <v>1064</v>
       </c>
       <c r="D10" s="3">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1187</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3">
-        <v>773</v>
+        <v>805</v>
       </c>
       <c r="C11" s="3">
-        <v>728</v>
+        <v>712</v>
       </c>
       <c r="D11" s="3">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2721</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3">
+        <v>506</v>
+      </c>
+      <c r="C12" s="3">
         <v>497</v>
       </c>
-      <c r="C12" s="3">
-        <v>469</v>
-      </c>
       <c r="D12" s="3">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4968</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5971</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="3">
-        <v>739</v>
+        <v>686</v>
       </c>
       <c r="C13" s="3">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="D13" s="3">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9384</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <v>19240</v>
+        <v>18817</v>
       </c>
       <c r="C14" s="3">
-        <v>17215</v>
+        <v>17079</v>
       </c>
       <c r="D14" s="3">
-        <v>36455</v>
+        <v>71572</v>
+      </c>
+      <c r="E14" s="3">
+        <v>107468</v>
       </c>
     </row>
   </sheetData>
@@ -4863,10 +6230,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,14 +6241,14 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -4898,26 +6265,29 @@
     <col min="25" max="25" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4933,14 +6303,20 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
-        <v>1294</v>
+        <v>1306</v>
       </c>
       <c r="D4" s="3">
         <v>52</v>
@@ -4948,20 +6324,24 @@
       <c r="E4" s="3">
         <v>213</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>2100</v>
+      </c>
+      <c r="H4" s="3">
         <v>52</v>
       </c>
-      <c r="G4" s="3">
-        <v>1507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="3">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
-        <v>1477</v>
+        <v>1490</v>
       </c>
       <c r="D5" s="3">
         <v>73</v>
@@ -4969,20 +6349,24 @@
       <c r="E5" s="3">
         <v>102</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>836</v>
+      </c>
+      <c r="H5" s="3">
         <v>73</v>
       </c>
-      <c r="G5" s="3">
-        <v>1579</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="3">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
-        <v>1120</v>
+        <v>1256</v>
       </c>
       <c r="D6" s="3">
         <v>503</v>
@@ -4990,20 +6374,24 @@
       <c r="E6" s="3">
         <v>1038</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>2454</v>
+      </c>
+      <c r="H6" s="3">
         <v>503</v>
       </c>
-      <c r="G6" s="3">
-        <v>2158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
-        <v>1441</v>
+        <v>1480</v>
       </c>
       <c r="D7" s="3">
         <v>422</v>
@@ -5011,14 +6399,18 @@
       <c r="E7" s="3">
         <v>849</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>1588</v>
+      </c>
+      <c r="H7" s="3">
         <v>422</v>
       </c>
-      <c r="G7" s="3">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="3">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -5030,41 +6422,49 @@
       <c r="E8" s="3">
         <v>2077</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>12315</v>
+      </c>
+      <c r="H8" s="3">
         <v>991</v>
       </c>
-      <c r="G8" s="3">
-        <v>2077</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <v>14392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
-        <v>3930</v>
+        <v>3908</v>
       </c>
       <c r="D9" s="3">
-        <v>950</v>
+        <v>995</v>
       </c>
       <c r="E9" s="3">
         <v>1708</v>
       </c>
-      <c r="F9" s="3">
-        <v>950</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3">
-        <v>5638</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21160</v>
+      </c>
+      <c r="H9" s="3">
+        <v>995</v>
+      </c>
+      <c r="I9" s="3">
+        <v>26776</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
-        <v>3133</v>
+        <v>3158</v>
       </c>
       <c r="D10" s="3">
         <v>769</v>
@@ -5072,39 +6472,47 @@
       <c r="E10" s="3">
         <v>1995</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>12269</v>
+      </c>
+      <c r="H10" s="3">
         <v>769</v>
       </c>
-      <c r="G10" s="3">
-        <v>5128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <v>17422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
-        <v>1316</v>
+        <v>1325</v>
       </c>
       <c r="E11" s="3">
         <v>1693</v>
       </c>
-      <c r="F11" s="3">
-        <v>1316</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2686</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1325</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>3793</v>
+        <v>3859</v>
       </c>
       <c r="D12" s="3">
         <v>1473</v>
@@ -5112,20 +6520,24 @@
       <c r="E12" s="3">
         <v>2597</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>7181</v>
+      </c>
+      <c r="H12" s="3">
         <v>1473</v>
       </c>
-      <c r="G12" s="3">
-        <v>6390</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>13637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>2827</v>
+        <v>2831</v>
       </c>
       <c r="D13" s="3">
         <v>957</v>
@@ -5133,53 +6545,65 @@
       <c r="E13" s="3">
         <v>1723</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>16006</v>
+      </c>
+      <c r="H13" s="3">
         <v>957</v>
       </c>
-      <c r="G13" s="3">
-        <v>4550</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="3">
+        <v>20560</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
-        <v>2195</v>
+        <v>2205</v>
       </c>
       <c r="D14" s="3">
-        <v>941</v>
+        <v>961</v>
       </c>
       <c r="E14" s="3">
         <v>1751</v>
       </c>
-      <c r="F14" s="3">
-        <v>941</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3">
-        <v>3946</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15297</v>
+      </c>
+      <c r="H14" s="3">
+        <v>961</v>
+      </c>
+      <c r="I14" s="3">
+        <v>19253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
-        <v>21210</v>
+        <v>21493</v>
       </c>
       <c r="D15" s="3">
-        <v>8447</v>
+        <v>8521</v>
       </c>
       <c r="E15" s="3">
         <v>15746</v>
       </c>
-      <c r="F15" s="3">
-        <v>8447</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3">
-        <v>36956</v>
+        <v>93892</v>
+      </c>
+      <c r="H15" s="3">
+        <v>8521</v>
+      </c>
+      <c r="I15" s="3">
+        <v>131131</v>
       </c>
     </row>
   </sheetData>
@@ -5190,10 +6614,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5201,14 +6625,14 @@
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -5225,26 +6649,29 @@
     <col min="25" max="25" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -5260,35 +6687,45 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
-        <v>36206</v>
+        <v>35410</v>
       </c>
       <c r="D4" s="3">
         <v>2193</v>
       </c>
       <c r="E4" s="3">
-        <v>7110</v>
-      </c>
-      <c r="F4" s="3">
+        <v>7006</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>93677</v>
+      </c>
+      <c r="H4" s="3">
         <v>2193</v>
       </c>
-      <c r="G4" s="3">
-        <v>43316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="3">
+        <v>136093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
-        <v>44207</v>
+        <v>46748</v>
       </c>
       <c r="D5" s="3">
         <v>3051</v>
@@ -5296,20 +6733,24 @@
       <c r="E5" s="3">
         <v>695</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>36186</v>
+      </c>
+      <c r="H5" s="3">
         <v>3051</v>
       </c>
-      <c r="G5" s="3">
-        <v>44902</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="3">
+        <v>83629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
-        <v>9791</v>
+        <v>12673</v>
       </c>
       <c r="D6" s="3">
         <v>605</v>
@@ -5317,35 +6758,43 @@
       <c r="E6" s="3">
         <v>3213</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>20147</v>
+      </c>
+      <c r="H6" s="3">
         <v>605</v>
       </c>
-      <c r="G6" s="3">
-        <v>13004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <v>36033</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
-        <v>12093</v>
+        <v>13186</v>
       </c>
       <c r="D7" s="3">
-        <v>703</v>
+        <v>652</v>
       </c>
       <c r="E7" s="3">
         <v>3625</v>
       </c>
-      <c r="F7" s="3">
-        <v>703</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3">
-        <v>15718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5838</v>
+      </c>
+      <c r="H7" s="3">
+        <v>652</v>
+      </c>
+      <c r="I7" s="3">
+        <v>22649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -5357,20 +6806,24 @@
       <c r="E8" s="3">
         <v>26094</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>298963</v>
+      </c>
+      <c r="H8" s="3">
         <v>17217</v>
       </c>
-      <c r="G8" s="3">
-        <v>26094</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <v>325057</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
-        <v>72376</v>
+        <v>70935</v>
       </c>
       <c r="D9" s="3">
         <v>32380</v>
@@ -5378,20 +6831,24 @@
       <c r="E9" s="3">
         <v>44228</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>23924</v>
+      </c>
+      <c r="H9" s="3">
         <v>32380</v>
       </c>
-      <c r="G9" s="3">
-        <v>116604</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="3">
+        <v>139087</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
-        <v>47318</v>
+        <v>51564</v>
       </c>
       <c r="D10" s="3">
         <v>16973</v>
@@ -5399,14 +6856,18 @@
       <c r="E10" s="3">
         <v>25812</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>281792</v>
+      </c>
+      <c r="H10" s="3">
         <v>16973</v>
       </c>
-      <c r="G10" s="3">
-        <v>73130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <v>359168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -5418,20 +6879,24 @@
       <c r="E11" s="3">
         <v>19017</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <v>202582</v>
+      </c>
+      <c r="H11" s="3">
         <v>12877</v>
       </c>
-      <c r="G11" s="3">
-        <v>19017</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="3">
+        <v>221599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>101261</v>
+        <v>106610</v>
       </c>
       <c r="D12" s="3">
         <v>37827</v>
@@ -5439,20 +6904,24 @@
       <c r="E12" s="3">
         <v>58402</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>650882</v>
+      </c>
+      <c r="H12" s="3">
         <v>37827</v>
       </c>
-      <c r="G12" s="3">
-        <v>159663</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>815894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>86261</v>
+        <v>113597</v>
       </c>
       <c r="D13" s="3">
         <v>31446</v>
@@ -5460,53 +6929,65 @@
       <c r="E13" s="3">
         <v>48448</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>563322</v>
+      </c>
+      <c r="H13" s="3">
         <v>31446</v>
       </c>
-      <c r="G13" s="3">
-        <v>134709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="3">
+        <v>725367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
-        <v>19787</v>
+        <v>19171</v>
       </c>
       <c r="D14" s="3">
-        <v>11758</v>
+        <v>10649</v>
       </c>
       <c r="E14" s="3">
         <v>15981</v>
       </c>
-      <c r="F14" s="3">
-        <v>11758</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3">
-        <v>35768</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>141763</v>
+      </c>
+      <c r="H14" s="3">
+        <v>10649</v>
+      </c>
+      <c r="I14" s="3">
+        <v>176915</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
-        <v>429300</v>
+        <v>469894</v>
       </c>
       <c r="D15" s="3">
-        <v>167030</v>
+        <v>165870</v>
       </c>
       <c r="E15" s="3">
-        <v>252625</v>
-      </c>
-      <c r="F15" s="3">
-        <v>167030</v>
-      </c>
+        <v>252521</v>
+      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3">
-        <v>681925</v>
+        <v>2319076</v>
+      </c>
+      <c r="H15" s="3">
+        <v>165870</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3041491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forced Hibernate to behave correctly.
Provided stateless session with explicit connection and managed setAutocommit and commit on it.
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -7,21 +7,20 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Unlicensed version" sheetId="7" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Simple" sheetId="2" r:id="rId3"/>
-    <sheet name="Standard" sheetId="3" r:id="rId4"/>
-    <sheet name="Complex" sheetId="6" r:id="rId5"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Simple" sheetId="2" r:id="rId2"/>
+    <sheet name="Standard" sheetId="3" r:id="rId3"/>
+    <sheet name="Complex" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="40" r:id="rId6"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="33">
   <si>
     <t>Simple</t>
   </si>
@@ -101,16 +100,6 @@
     <t>Npgsql</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Unlicensed version. Please register @ templater.info</t>
-    </r>
-  </si>
-  <si>
     <t>Revenj</t>
   </si>
   <si>
@@ -128,12 +117,15 @@
   <si>
     <t>Target filter</t>
   </si>
+  <si>
+    <t>Hibernate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,11 +133,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,6 +256,9 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="13"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="14"/>
@@ -280,6 +270,24 @@
         <c:idx val="16"/>
       </c:pivotFmt>
       <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
         <c:idx val="20"/>
         <c:marker>
           <c:symbol val="none"/>
@@ -299,18 +307,22 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="23"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="24"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="25"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
@@ -686,7 +698,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1257</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>796</c:v>
@@ -698,19 +710,112 @@
                   <c:v>5338</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1421</c:v>
+                  <c:v>1215</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1796</c:v>
+                  <c:v>1588</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>756</c:v>
+                  <c:v>678</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>692</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>858</c:v>
+                  <c:v>796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Simple!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hibernate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Simple!$A$5:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Bulk insert</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bulk update</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loop insert (half)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loop update (half)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Query all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Report (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Search all (x100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Query filter (x1.000)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Search subset (x3.000)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Find many (x2.000)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Find one (x5.000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Simple!$F$5:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5589</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2938</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3620</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1397</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,11 +830,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="174498560"/>
-        <c:axId val="174500096"/>
+        <c:axId val="168796928"/>
+        <c:axId val="168798464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="174498560"/>
+        <c:axId val="168796928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +843,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174500096"/>
+        <c:crossAx val="168798464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -746,7 +851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174500096"/>
+        <c:axId val="168798464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +882,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174498560"/>
+        <c:crossAx val="168796928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -849,7 +954,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1741,11 +1845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175333760"/>
-        <c:axId val="175335296"/>
+        <c:axId val="169450112"/>
+        <c:axId val="169451904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175333760"/>
+        <c:axId val="169450112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1754,7 +1858,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175335296"/>
+        <c:crossAx val="169451904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1762,7 +1866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175335296"/>
+        <c:axId val="169451904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,14 +1890,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175333760"/>
+        <c:crossAx val="169450112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1865,7 +1968,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2720,11 +2822,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175538176"/>
-        <c:axId val="175539712"/>
+        <c:axId val="182692480"/>
+        <c:axId val="182698368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175538176"/>
+        <c:axId val="182692480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2733,7 +2835,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175539712"/>
+        <c:crossAx val="182698368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2741,7 +2843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175539712"/>
+        <c:axId val="182698368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,14 +2867,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175538176"/>
+        <c:crossAx val="182692480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2915,7 +3016,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42151.969164467591" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42211.990716550928" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="55">
   <cacheSource type="worksheet">
     <worksheetSource name="Table3"/>
   </cacheSource>
@@ -2955,11 +3056,12 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="695" maxValue="650882"/>
     </cacheField>
     <cacheField name="Target" numFmtId="0">
-      <sharedItems count="9">
+      <sharedItems count="10">
         <s v="Npgsql"/>
         <s v="Revenj"/>
         <s v="Entity Framework"/>
         <s v="JDBC"/>
+        <s v="Hibernate"/>
         <s v="Revenj Postgres" u="1"/>
         <s v="MsSql ADO.NET" u="1"/>
         <s v="[[description]]" u="1"/>
@@ -2968,11 +3070,12 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Target filter" numFmtId="0">
-      <sharedItems count="4">
+      <sharedItems count="5">
         <s v="Npgsql"/>
         <s v="Revenj"/>
         <s v="Entity Framework"/>
         <s v="JDBC"/>
+        <s v="Hibernate"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2985,7 +3088,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="55">
   <r>
     <x v="0"/>
     <n v="1105"/>
@@ -3318,7 +3421,7 @@
   </r>
   <r>
     <x v="0"/>
-    <n v="1257"/>
+    <n v="900"/>
     <m/>
     <n v="580"/>
     <m/>
@@ -3358,7 +3461,7 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="1796"/>
+    <n v="1588"/>
     <m/>
     <n v="2385"/>
     <m/>
@@ -3368,7 +3471,7 @@
   </r>
   <r>
     <x v="5"/>
-    <n v="756"/>
+    <n v="678"/>
     <m/>
     <n v="3602"/>
     <m/>
@@ -3408,7 +3511,7 @@
   </r>
   <r>
     <x v="9"/>
-    <n v="858"/>
+    <n v="796"/>
     <m/>
     <n v="2304"/>
     <m/>
@@ -3418,20 +3521,130 @@
   </r>
   <r>
     <x v="10"/>
-    <n v="1421"/>
+    <n v="1215"/>
     <m/>
     <n v="4055"/>
     <m/>
     <m/>
     <x v="3"/>
     <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2467"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1945"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="5251"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="5589"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="3620"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1397"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="1002"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="1528"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="2938"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:E16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:F16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
       <items count="16">
@@ -3459,25 +3672,27 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="10">
+      <items count="11">
+        <item m="1" x="7"/>
         <item m="1" x="6"/>
+        <item x="0"/>
         <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
+        <item m="1" x="9"/>
         <item m="1" x="8"/>
-        <item m="1" x="7"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="4">
+      <items count="5">
         <item x="2"/>
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
+        <item x="4"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -3525,7 +3740,7 @@
   <colFields count="1">
     <field x="6"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="5">
     <i>
       <x v="2"/>
     </i>
@@ -3538,6 +3753,9 @@
     <i>
       <x v="8"/>
     </i>
+    <i>
+      <x v="9"/>
+    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="7" hier="-1"/>
@@ -3545,7 +3763,7 @@
   <dataFields count="1">
     <dataField name="Relational" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="21">
+  <chartFormats count="20">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3717,47 +3935,35 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="17" series="1">
+    <chartFormat chart="0" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="23" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="18" series="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="24" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
             <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="24" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3773,7 +3979,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" chartFormat="2">
   <location ref="A3:G17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -3802,25 +4008,27 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="10">
+      <items count="11">
+        <item m="1" x="7"/>
         <item m="1" x="6"/>
+        <item x="0"/>
         <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
+        <item m="1" x="9"/>
         <item m="1" x="8"/>
-        <item m="1" x="7"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="4">
+      <items count="5">
         <item h="1" x="2"/>
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
+        <item h="1" x="4"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -4358,7 +4566,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:G17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -4387,25 +4595,27 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="10">
+      <items count="11">
+        <item m="1" x="7"/>
         <item m="1" x="6"/>
+        <item x="0"/>
         <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
+        <item m="1" x="9"/>
         <item m="1" x="8"/>
-        <item m="1" x="7"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="4">
+      <items count="5">
         <item h="1" x="2"/>
         <item h="1" x="3"/>
         <item x="0"/>
         <item x="1"/>
+        <item h="1" x="4"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -4909,8 +5119,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H45" totalsRowShown="0">
-  <autoFilter ref="A1:H45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H56" totalsRowShown="0">
+  <autoFilter ref="A1:H56"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Bench type"/>
     <tableColumn id="2" name="Simple"/>
@@ -5212,27 +5422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5268,7 +5462,7 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5493,10 +5687,10 @@
         <v>7006</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5519,10 +5713,10 @@
         <v>695</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5545,10 +5739,10 @@
         <v>3213</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5571,10 +5765,10 @@
         <v>3597</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5597,10 +5791,10 @@
         <v>25592</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5623,10 +5817,10 @@
         <v>57687</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -5649,10 +5843,10 @@
         <v>26094</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5675,10 +5869,10 @@
         <v>19017</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5701,10 +5895,10 @@
         <v>48448</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5727,10 +5921,10 @@
         <v>15803</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5753,10 +5947,10 @@
         <v>44228</v>
       </c>
       <c r="G23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5773,10 +5967,10 @@
         <v>93677</v>
       </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5793,10 +5987,10 @@
         <v>36186</v>
       </c>
       <c r="G25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5813,10 +6007,10 @@
         <v>20147</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5833,10 +6027,10 @@
         <v>5838</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5853,10 +6047,10 @@
         <v>281792</v>
       </c>
       <c r="G28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5873,10 +6067,10 @@
         <v>650882</v>
       </c>
       <c r="G29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5893,10 +6087,10 @@
         <v>298963</v>
       </c>
       <c r="G30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -5913,10 +6107,10 @@
         <v>202582</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5933,10 +6127,10 @@
         <v>563322</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5953,10 +6147,10 @@
         <v>141763</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5973,10 +6167,10 @@
         <v>396652</v>
       </c>
       <c r="G34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5984,16 +6178,16 @@
         <v>5</v>
       </c>
       <c r="B35">
-        <v>1257</v>
+        <v>900</v>
       </c>
       <c r="D35">
         <v>580</v>
       </c>
       <c r="G35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,10 +6201,10 @@
         <v>738</v>
       </c>
       <c r="G36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -6024,10 +6218,10 @@
         <v>988</v>
       </c>
       <c r="G37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -6041,10 +6235,10 @@
         <v>1249</v>
       </c>
       <c r="G38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6052,16 +6246,16 @@
         <v>9</v>
       </c>
       <c r="B39">
-        <v>1796</v>
+        <v>1588</v>
       </c>
       <c r="D39">
         <v>2385</v>
       </c>
       <c r="G39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6069,16 +6263,16 @@
         <v>22</v>
       </c>
       <c r="B40">
-        <v>756</v>
+        <v>678</v>
       </c>
       <c r="D40">
         <v>3602</v>
       </c>
       <c r="G40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -6086,10 +6280,10 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -6097,10 +6291,10 @@
         <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -6114,10 +6308,10 @@
         <v>2479</v>
       </c>
       <c r="G43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6125,16 +6319,16 @@
         <v>24</v>
       </c>
       <c r="B44">
-        <v>858</v>
+        <v>796</v>
       </c>
       <c r="D44">
         <v>2304</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -6142,16 +6336,164 @@
         <v>11</v>
       </c>
       <c r="B45">
-        <v>1421</v>
+        <v>1215</v>
       </c>
       <c r="D45">
         <v>4055</v>
       </c>
       <c r="G45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H45" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>2467</v>
+      </c>
+      <c r="G46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>1945</v>
+      </c>
+      <c r="G47" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>5251</v>
+      </c>
+      <c r="G48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>5589</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>3620</v>
+      </c>
+      <c r="G50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51">
+        <v>1397</v>
+      </c>
+      <c r="G51" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" t="s">
+        <v>32</v>
+      </c>
+      <c r="H53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54">
+        <v>1002</v>
+      </c>
+      <c r="G54" t="s">
+        <v>32</v>
+      </c>
+      <c r="H54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <v>1528</v>
+      </c>
+      <c r="G55" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>2938</v>
+      </c>
+      <c r="G56" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -6163,12 +6505,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6178,7 +6520,7 @@
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
@@ -6199,15 +6541,15 @@
     <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -6215,7 +6557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -6223,16 +6565,19 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -6246,10 +6591,13 @@
         <v>3119</v>
       </c>
       <c r="E5" s="3">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -6265,8 +6613,11 @@
       <c r="E6" s="3">
         <v>796</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -6282,8 +6633,11 @@
       <c r="E7" s="3">
         <v>5148</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>5251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -6299,8 +6653,11 @@
       <c r="E8" s="3">
         <v>5338</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>5589</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -6312,8 +6669,9 @@
         <v>2305</v>
       </c>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -6327,10 +6685,13 @@
         <v>17136</v>
       </c>
       <c r="E10" s="3">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1215</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -6344,10 +6705,13 @@
         <v>2288</v>
       </c>
       <c r="E11" s="3">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1588</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -6359,8 +6723,9 @@
         <v>1187</v>
       </c>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -6374,10 +6739,13 @@
         <v>2721</v>
       </c>
       <c r="E13" s="3">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -6393,8 +6761,11 @@
       <c r="E14" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -6408,10 +6779,13 @@
         <v>9384</v>
       </c>
       <c r="E15" s="3">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>796</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -6425,7 +6799,10 @@
         <v>71572</v>
       </c>
       <c r="E16" s="3">
-        <v>18062</v>
+        <v>17151</v>
+      </c>
+      <c r="F16" s="3">
+        <v>25737</v>
       </c>
     </row>
   </sheetData>
@@ -6434,9 +6811,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
@@ -6473,10 +6850,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6489,10 +6866,10 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6745,7 +7122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -6784,10 +7161,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6800,7 +7177,7 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Revenj.NET v1.2.1, latest Postgres JDBC driver.
Updated results.
JDBC seems much faster at reading now ;)
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -641,25 +641,25 @@
                   <c:v>796</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5148</c:v>
+                  <c:v>4593</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5338</c:v>
+                  <c:v>4622</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1215</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1588</c:v>
+                  <c:v>767</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>678</c:v>
+                  <c:v>556</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>692</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>796</c:v>
+                  <c:v>428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -852,7 +852,7 @@
                   <c:v>1487</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1064</c:v>
+                  <c:v>988</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>712</c:v>
@@ -861,7 +861,7 @@
                   <c:v>376</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>509</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,34 +935,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>176</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>232</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4640</c:v>
+                  <c:v>4636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4855</c:v>
+                  <c:v>4798</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1767</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>642</c:v>
+                  <c:v>602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1933</c:v>
+                  <c:v>1753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2169</c:v>
+                  <c:v>2074</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>970</c:v>
+                  <c:v>878</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>615</c:v>
+                  <c:v>599</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>866</c:v>
@@ -980,11 +980,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106368000"/>
-        <c:axId val="106386176"/>
+        <c:axId val="48551808"/>
+        <c:axId val="48553344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106368000"/>
+        <c:axId val="48551808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +993,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106386176"/>
+        <c:crossAx val="48553344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1001,7 +1001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106386176"/>
+        <c:axId val="48553344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8000"/>
@@ -1033,7 +1033,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106368000"/>
+        <c:crossAx val="48551808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1991,25 +1991,25 @@
                   <c:v>738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>988</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1249</c:v>
+                  <c:v>894</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4055</c:v>
+                  <c:v>1753</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2385</c:v>
+                  <c:v>2187</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3602</c:v>
+                  <c:v>1943</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2479</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2304</c:v>
+                  <c:v>1033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2262,22 +2262,22 @@
                   <c:v>991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>995</c:v>
+                  <c:v>994</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>769</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1325</c:v>
+                  <c:v>1236</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1469</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>957</c:v>
+                  <c:v>915</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>750</c:v>
+                  <c:v>672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2375,7 +2375,7 @@
                   <c:v>1944</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1693</c:v>
+                  <c:v>1673</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2597</c:v>
@@ -2384,7 +2384,7 @@
                   <c:v>1723</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>982</c:v>
+                  <c:v>917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2461,28 +2461,28 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>531</c:v>
+                  <c:v>527</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>545</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>879</c:v>
+                  <c:v>876</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1298</c:v>
+                  <c:v>1188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1012</c:v>
+                  <c:v>964</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1004</c:v>
+                  <c:v>975</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1450</c:v>
+                  <c:v>1289</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1034</c:v>
@@ -2565,10 +2565,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>464</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1125</c:v>
@@ -2577,25 +2577,25 @@
                   <c:v>1120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2105</c:v>
+                  <c:v>2188</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2011</c:v>
+                  <c:v>1923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2271</c:v>
+                  <c:v>2255</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1404</c:v>
+                  <c:v>1401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2687</c:v>
+                  <c:v>2560</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2154</c:v>
+                  <c:v>2096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2023</c:v>
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2610,11 +2610,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106885504"/>
-        <c:axId val="106887040"/>
+        <c:axId val="48585728"/>
+        <c:axId val="48599808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106885504"/>
+        <c:axId val="48585728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2623,7 +2623,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106887040"/>
+        <c:crossAx val="48599808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2631,7 +2631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106887040"/>
+        <c:axId val="48599808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2663,7 +2663,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106885504"/>
+        <c:crossAx val="48585728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2735,6 +2735,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3697,10 +3698,10 @@
                   <c:v>37437</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31446</c:v>
+                  <c:v>23711</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9549</c:v>
+                  <c:v>7274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3786,7 +3787,7 @@
                   <c:v>3213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3597</c:v>
+                  <c:v>3499</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>26094</c:v>
@@ -3804,10 +3805,10 @@
                   <c:v>57687</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48448</c:v>
+                  <c:v>36165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15803</c:v>
+                  <c:v>10745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4033,11 +4034,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106902656"/>
-        <c:axId val="106904192"/>
+        <c:axId val="49217536"/>
+        <c:axId val="49219072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106902656"/>
+        <c:axId val="49217536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4046,7 +4047,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106904192"/>
+        <c:crossAx val="49219072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4054,7 +4055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106904192"/>
+        <c:axId val="49219072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150000"/>
@@ -4079,13 +4080,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106902656"/>
+        <c:crossAx val="49217536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4228,7 +4230,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42236.096996412038" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="66">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42261.640310995368" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="66">
   <cacheSource type="worksheet">
     <worksheetSource name="Table3"/>
   </cacheSource>
@@ -4451,7 +4453,7 @@
     <n v="422"/>
     <n v="849"/>
     <n v="652"/>
-    <n v="3597"/>
+    <n v="3499"/>
     <x v="1"/>
     <x v="1"/>
   </r>
@@ -4487,9 +4489,9 @@
   </r>
   <r>
     <x v="7"/>
-    <n v="1064"/>
-    <n v="1325"/>
-    <n v="1693"/>
+    <n v="988"/>
+    <n v="1236"/>
+    <n v="1673"/>
     <n v="12877"/>
     <n v="19017"/>
     <x v="1"/>
@@ -4498,27 +4500,27 @@
   <r>
     <x v="8"/>
     <n v="376"/>
-    <n v="957"/>
+    <n v="915"/>
     <n v="1723"/>
-    <n v="31446"/>
-    <n v="48448"/>
+    <n v="23711"/>
+    <n v="36165"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="9"/>
-    <n v="509"/>
-    <n v="750"/>
-    <n v="982"/>
-    <n v="9549"/>
-    <n v="15803"/>
+    <n v="475"/>
+    <n v="672"/>
+    <n v="917"/>
+    <n v="7274"/>
+    <n v="10745"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <x v="10"/>
     <n v="402"/>
-    <n v="995"/>
+    <n v="994"/>
     <n v="1708"/>
     <n v="32380"/>
     <n v="44228"/>
@@ -4657,9 +4659,9 @@
   </r>
   <r>
     <x v="2"/>
-    <n v="5148"/>
-    <m/>
-    <n v="988"/>
+    <n v="4593"/>
+    <m/>
+    <n v="856"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4667,9 +4669,9 @@
   </r>
   <r>
     <x v="3"/>
-    <n v="5338"/>
-    <m/>
-    <n v="1249"/>
+    <n v="4622"/>
+    <m/>
+    <n v="894"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4677,9 +4679,9 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="1588"/>
-    <m/>
-    <n v="2385"/>
+    <n v="767"/>
+    <m/>
+    <n v="2187"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4687,9 +4689,9 @@
   </r>
   <r>
     <x v="5"/>
-    <n v="678"/>
-    <m/>
-    <n v="3602"/>
+    <n v="556"/>
+    <m/>
+    <n v="1943"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4717,9 +4719,9 @@
   </r>
   <r>
     <x v="8"/>
-    <n v="692"/>
-    <m/>
-    <n v="2479"/>
+    <n v="463"/>
+    <m/>
+    <n v="1600"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4727,9 +4729,9 @@
   </r>
   <r>
     <x v="9"/>
-    <n v="796"/>
-    <m/>
-    <n v="2304"/>
+    <n v="428"/>
+    <m/>
+    <n v="1033"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4737,9 +4739,9 @@
   </r>
   <r>
     <x v="10"/>
-    <n v="1215"/>
-    <m/>
-    <n v="4055"/>
+    <n v="645"/>
+    <m/>
+    <n v="1753"/>
     <m/>
     <m/>
     <x v="3"/>
@@ -4857,9 +4859,9 @@
   </r>
   <r>
     <x v="0"/>
-    <n v="176"/>
+    <n v="146"/>
     <n v="52"/>
-    <n v="464"/>
+    <n v="272"/>
     <n v="1929"/>
     <n v="8500"/>
     <x v="5"/>
@@ -4867,9 +4869,9 @@
   </r>
   <r>
     <x v="1"/>
-    <n v="232"/>
-    <n v="94"/>
-    <n v="157"/>
+    <n v="224"/>
+    <n v="86"/>
+    <n v="148"/>
     <n v="3976"/>
     <n v="9722"/>
     <x v="5"/>
@@ -4877,8 +4879,8 @@
   </r>
   <r>
     <x v="2"/>
-    <n v="4640"/>
-    <n v="531"/>
+    <n v="4636"/>
+    <n v="527"/>
     <n v="1125"/>
     <n v="515"/>
     <n v="3944"/>
@@ -4887,7 +4889,7 @@
   </r>
   <r>
     <x v="3"/>
-    <n v="4855"/>
+    <n v="4798"/>
     <n v="545"/>
     <n v="1120"/>
     <n v="808"/>
@@ -4897,9 +4899,9 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="1933"/>
-    <n v="1012"/>
-    <n v="2271"/>
+    <n v="1753"/>
+    <n v="964"/>
+    <n v="2255"/>
     <n v="19010"/>
     <n v="29012"/>
     <x v="5"/>
@@ -4907,9 +4909,9 @@
   </r>
   <r>
     <x v="5"/>
-    <n v="970"/>
-    <n v="1450"/>
-    <n v="2687"/>
+    <n v="878"/>
+    <n v="1289"/>
+    <n v="2560"/>
     <n v="42673"/>
     <n v="65443"/>
     <x v="5"/>
@@ -4918,8 +4920,8 @@
   <r>
     <x v="6"/>
     <n v="1767"/>
-    <n v="879"/>
-    <n v="2105"/>
+    <n v="876"/>
+    <n v="2188"/>
     <n v="18569"/>
     <n v="28668"/>
     <x v="5"/>
@@ -4927,9 +4929,9 @@
   </r>
   <r>
     <x v="7"/>
-    <n v="2169"/>
-    <n v="1004"/>
-    <n v="1404"/>
+    <n v="2074"/>
+    <n v="975"/>
+    <n v="1401"/>
     <n v="14307"/>
     <n v="21756"/>
     <x v="5"/>
@@ -4937,9 +4939,9 @@
   </r>
   <r>
     <x v="8"/>
-    <n v="615"/>
+    <n v="599"/>
     <n v="1034"/>
-    <n v="2154"/>
+    <n v="2096"/>
     <n v="26137"/>
     <n v="41396"/>
     <x v="5"/>
@@ -4949,7 +4951,7 @@
     <x v="9"/>
     <n v="866"/>
     <n v="1139"/>
-    <n v="2023"/>
+    <n v="2017"/>
     <n v="7537"/>
     <n v="12818"/>
     <x v="5"/>
@@ -4957,9 +4959,9 @@
   </r>
   <r>
     <x v="10"/>
-    <n v="642"/>
-    <n v="1298"/>
-    <n v="2011"/>
+    <n v="602"/>
+    <n v="1188"/>
+    <n v="1923"/>
     <n v="34088"/>
     <n v="51141"/>
     <x v="5"/>
@@ -6965,7 +6967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7301,7 +7305,7 @@
         <v>652</v>
       </c>
       <c r="F16">
-        <v>3597</v>
+        <v>3499</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
@@ -7393,13 +7397,13 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>1064</v>
+        <v>988</v>
       </c>
       <c r="C20">
-        <v>1325</v>
+        <v>1236</v>
       </c>
       <c r="D20">
-        <v>1693</v>
+        <v>1673</v>
       </c>
       <c r="E20">
         <v>12877</v>
@@ -7422,16 +7426,16 @@
         <v>376</v>
       </c>
       <c r="C21">
-        <v>957</v>
+        <v>915</v>
       </c>
       <c r="D21">
         <v>1723</v>
       </c>
       <c r="E21">
-        <v>31446</v>
+        <v>23711</v>
       </c>
       <c r="F21">
-        <v>48448</v>
+        <v>36165</v>
       </c>
       <c r="G21" t="s">
         <v>31</v>
@@ -7445,19 +7449,19 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>509</v>
+        <v>475</v>
       </c>
       <c r="C22">
-        <v>750</v>
+        <v>672</v>
       </c>
       <c r="D22">
-        <v>982</v>
+        <v>917</v>
       </c>
       <c r="E22">
-        <v>9549</v>
+        <v>7274</v>
       </c>
       <c r="F22">
-        <v>15803</v>
+        <v>10745</v>
       </c>
       <c r="G22" t="s">
         <v>31</v>
@@ -7474,7 +7478,7 @@
         <v>402</v>
       </c>
       <c r="C23">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D23">
         <v>1708</v>
@@ -7751,10 +7755,10 @@
         <v>7</v>
       </c>
       <c r="B37">
-        <v>5148</v>
+        <v>4593</v>
       </c>
       <c r="D37">
-        <v>988</v>
+        <v>856</v>
       </c>
       <c r="G37" t="s">
         <v>27</v>
@@ -7768,10 +7772,10 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <v>5338</v>
+        <v>4622</v>
       </c>
       <c r="D38">
-        <v>1249</v>
+        <v>894</v>
       </c>
       <c r="G38" t="s">
         <v>27</v>
@@ -7785,10 +7789,10 @@
         <v>9</v>
       </c>
       <c r="B39">
-        <v>1588</v>
+        <v>767</v>
       </c>
       <c r="D39">
-        <v>2385</v>
+        <v>2187</v>
       </c>
       <c r="G39" t="s">
         <v>27</v>
@@ -7802,10 +7806,10 @@
         <v>22</v>
       </c>
       <c r="B40">
-        <v>678</v>
+        <v>556</v>
       </c>
       <c r="D40">
-        <v>3602</v>
+        <v>1943</v>
       </c>
       <c r="G40" t="s">
         <v>27</v>
@@ -7841,10 +7845,10 @@
         <v>23</v>
       </c>
       <c r="B43">
-        <v>692</v>
+        <v>463</v>
       </c>
       <c r="D43">
-        <v>2479</v>
+        <v>1600</v>
       </c>
       <c r="G43" t="s">
         <v>27</v>
@@ -7858,10 +7862,10 @@
         <v>24</v>
       </c>
       <c r="B44">
-        <v>796</v>
+        <v>428</v>
       </c>
       <c r="D44">
-        <v>2304</v>
+        <v>1033</v>
       </c>
       <c r="G44" t="s">
         <v>27</v>
@@ -7875,10 +7879,10 @@
         <v>11</v>
       </c>
       <c r="B45">
-        <v>1215</v>
+        <v>645</v>
       </c>
       <c r="D45">
-        <v>4055</v>
+        <v>1753</v>
       </c>
       <c r="G45" t="s">
         <v>27</v>
@@ -8067,13 +8071,13 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="C57">
         <v>52</v>
       </c>
       <c r="D57">
-        <v>464</v>
+        <v>272</v>
       </c>
       <c r="E57">
         <v>1929</v>
@@ -8093,13 +8097,13 @@
         <v>6</v>
       </c>
       <c r="B58">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C58">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D58">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E58">
         <v>3976</v>
@@ -8119,10 +8123,10 @@
         <v>7</v>
       </c>
       <c r="B59">
-        <v>4640</v>
+        <v>4636</v>
       </c>
       <c r="C59">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D59">
         <v>1125</v>
@@ -8145,7 +8149,7 @@
         <v>8</v>
       </c>
       <c r="B60">
-        <v>4855</v>
+        <v>4798</v>
       </c>
       <c r="C60">
         <v>545</v>
@@ -8171,13 +8175,13 @@
         <v>9</v>
       </c>
       <c r="B61">
-        <v>1933</v>
+        <v>1753</v>
       </c>
       <c r="C61">
-        <v>1012</v>
+        <v>964</v>
       </c>
       <c r="D61">
-        <v>2271</v>
+        <v>2255</v>
       </c>
       <c r="E61">
         <v>19010</v>
@@ -8197,13 +8201,13 @@
         <v>22</v>
       </c>
       <c r="B62">
-        <v>970</v>
+        <v>878</v>
       </c>
       <c r="C62">
-        <v>1450</v>
+        <v>1289</v>
       </c>
       <c r="D62">
-        <v>2687</v>
+        <v>2560</v>
       </c>
       <c r="E62">
         <v>42673</v>
@@ -8226,10 +8230,10 @@
         <v>1767</v>
       </c>
       <c r="C63">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="D63">
-        <v>2105</v>
+        <v>2188</v>
       </c>
       <c r="E63">
         <v>18569</v>
@@ -8249,13 +8253,13 @@
         <v>17</v>
       </c>
       <c r="B64">
-        <v>2169</v>
+        <v>2074</v>
       </c>
       <c r="C64">
-        <v>1004</v>
+        <v>975</v>
       </c>
       <c r="D64">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="E64">
         <v>14307</v>
@@ -8275,13 +8279,13 @@
         <v>23</v>
       </c>
       <c r="B65">
-        <v>615</v>
+        <v>599</v>
       </c>
       <c r="C65">
         <v>1034</v>
       </c>
       <c r="D65">
-        <v>2154</v>
+        <v>2096</v>
       </c>
       <c r="E65">
         <v>26137</v>
@@ -8307,7 +8311,7 @@
         <v>1139</v>
       </c>
       <c r="D66">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="E66">
         <v>7537</v>
@@ -8327,13 +8331,13 @@
         <v>11</v>
       </c>
       <c r="B67">
-        <v>642</v>
+        <v>602</v>
       </c>
       <c r="C67">
-        <v>1298</v>
+        <v>1188</v>
       </c>
       <c r="D67">
-        <v>2011</v>
+        <v>1923</v>
       </c>
       <c r="E67">
         <v>34088</v>
@@ -8361,8 +8365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8452,7 +8456,7 @@
         <v>123</v>
       </c>
       <c r="G5" s="3">
-        <v>176</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -8475,7 +8479,7 @@
         <v>210</v>
       </c>
       <c r="G6" s="3">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -8489,7 +8493,7 @@
         <v>12331</v>
       </c>
       <c r="D7" s="3">
-        <v>5148</v>
+        <v>4593</v>
       </c>
       <c r="E7" s="3">
         <v>9960</v>
@@ -8498,7 +8502,7 @@
         <v>4632</v>
       </c>
       <c r="G7" s="3">
-        <v>4640</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -8512,7 +8516,7 @@
         <v>13345</v>
       </c>
       <c r="D8" s="3">
-        <v>5338</v>
+        <v>4622</v>
       </c>
       <c r="E8" s="3">
         <v>7008</v>
@@ -8521,7 +8525,7 @@
         <v>4689</v>
       </c>
       <c r="G8" s="3">
-        <v>4855</v>
+        <v>4798</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -8552,7 +8556,7 @@
         <v>17136</v>
       </c>
       <c r="D10" s="3">
-        <v>1215</v>
+        <v>645</v>
       </c>
       <c r="E10" s="3">
         <v>2564</v>
@@ -8561,7 +8565,7 @@
         <v>402</v>
       </c>
       <c r="G10" s="3">
-        <v>642</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -8575,7 +8579,7 @@
         <v>2288</v>
       </c>
       <c r="D11" s="3">
-        <v>1588</v>
+        <v>767</v>
       </c>
       <c r="E11" s="3">
         <v>3765</v>
@@ -8584,7 +8588,7 @@
         <v>1487</v>
       </c>
       <c r="G11" s="3">
-        <v>1933</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -8598,10 +8602,10 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3">
-        <v>1064</v>
+        <v>988</v>
       </c>
       <c r="G12" s="3">
-        <v>2169</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -8615,7 +8619,7 @@
         <v>2721</v>
       </c>
       <c r="D13" s="3">
-        <v>678</v>
+        <v>556</v>
       </c>
       <c r="E13" s="3">
         <v>1443</v>
@@ -8624,7 +8628,7 @@
         <v>712</v>
       </c>
       <c r="G13" s="3">
-        <v>970</v>
+        <v>878</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -8638,7 +8642,7 @@
         <v>4968</v>
       </c>
       <c r="D14" s="3">
-        <v>692</v>
+        <v>463</v>
       </c>
       <c r="E14" s="3">
         <v>1039</v>
@@ -8647,7 +8651,7 @@
         <v>376</v>
       </c>
       <c r="G14" s="3">
-        <v>615</v>
+        <v>599</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -8661,13 +8665,13 @@
         <v>9384</v>
       </c>
       <c r="D15" s="3">
-        <v>796</v>
+        <v>428</v>
       </c>
       <c r="E15" s="3">
         <v>1215</v>
       </c>
       <c r="F15" s="3">
-        <v>509</v>
+        <v>475</v>
       </c>
       <c r="G15" s="3">
         <v>866</v>
@@ -8684,16 +8688,16 @@
         <v>71572</v>
       </c>
       <c r="D16" s="3">
-        <v>17151</v>
+        <v>13770</v>
       </c>
       <c r="E16" s="3">
         <v>33475</v>
       </c>
       <c r="F16" s="3">
-        <v>16187</v>
+        <v>16077</v>
       </c>
       <c r="G16" s="3">
-        <v>18865</v>
+        <v>18343</v>
       </c>
     </row>
   </sheetData>
@@ -8706,8 +8710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8843,7 +8847,7 @@
         <v>52</v>
       </c>
       <c r="M6" s="3">
-        <v>464</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -8873,10 +8877,10 @@
         <v>95</v>
       </c>
       <c r="L7" s="3">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="M7" s="3">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -8893,7 +8897,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3">
-        <v>988</v>
+        <v>856</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
@@ -8906,7 +8910,7 @@
         <v>964</v>
       </c>
       <c r="L8" s="3">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="M8" s="3">
         <v>1125</v>
@@ -8926,7 +8930,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3">
-        <v>1249</v>
+        <v>894</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3">
@@ -8966,10 +8970,10 @@
         <v>2062</v>
       </c>
       <c r="L10" s="3">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="M10" s="3">
-        <v>2105</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -8986,23 +8990,23 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>4055</v>
+        <v>1753</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3">
         <v>7193</v>
       </c>
       <c r="J11" s="3">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="K11" s="3">
         <v>1708</v>
       </c>
       <c r="L11" s="3">
-        <v>1298</v>
+        <v>1188</v>
       </c>
       <c r="M11" s="3">
-        <v>2011</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -9019,7 +9023,7 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3">
-        <v>2385</v>
+        <v>2187</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
@@ -9032,10 +9036,10 @@
         <v>1944</v>
       </c>
       <c r="L12" s="3">
-        <v>1012</v>
+        <v>964</v>
       </c>
       <c r="M12" s="3">
-        <v>2271</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -9053,16 +9057,16 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3">
-        <v>1325</v>
+        <v>1236</v>
       </c>
       <c r="K13" s="3">
-        <v>1693</v>
+        <v>1673</v>
       </c>
       <c r="L13" s="3">
-        <v>1004</v>
+        <v>975</v>
       </c>
       <c r="M13" s="3">
-        <v>1404</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -9079,7 +9083,7 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3">
-        <v>3602</v>
+        <v>1943</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3">
@@ -9092,10 +9096,10 @@
         <v>2597</v>
       </c>
       <c r="L14" s="3">
-        <v>1450</v>
+        <v>1289</v>
       </c>
       <c r="M14" s="3">
-        <v>2687</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -9112,14 +9116,14 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3">
-        <v>2479</v>
+        <v>1600</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
         <v>7713</v>
       </c>
       <c r="J15" s="3">
-        <v>957</v>
+        <v>915</v>
       </c>
       <c r="K15" s="3">
         <v>1723</v>
@@ -9128,7 +9132,7 @@
         <v>1034</v>
       </c>
       <c r="M15" s="3">
-        <v>2154</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -9145,23 +9149,23 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3">
-        <v>2304</v>
+        <v>1033</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
         <v>14400</v>
       </c>
       <c r="J16" s="3">
-        <v>750</v>
+        <v>672</v>
       </c>
       <c r="K16" s="3">
-        <v>982</v>
+        <v>917</v>
       </c>
       <c r="L16" s="3">
         <v>1139</v>
       </c>
       <c r="M16" s="3">
-        <v>2023</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -9178,23 +9182,23 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3">
-        <v>18380</v>
+        <v>11584</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
         <v>78813</v>
       </c>
       <c r="J17" s="3">
-        <v>8247</v>
+        <v>8037</v>
       </c>
       <c r="K17" s="3">
-        <v>14818</v>
+        <v>14733</v>
       </c>
       <c r="L17" s="3">
-        <v>9038</v>
+        <v>8675</v>
       </c>
       <c r="M17" s="3">
-        <v>17521</v>
+        <v>17105</v>
       </c>
     </row>
   </sheetData>
@@ -9208,8 +9212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9412,7 +9416,7 @@
         <v>652</v>
       </c>
       <c r="G9" s="3">
-        <v>3597</v>
+        <v>3499</v>
       </c>
       <c r="H9" s="3">
         <v>808</v>
@@ -9424,7 +9428,7 @@
         <v>1460</v>
       </c>
       <c r="K9" s="3">
-        <v>24448</v>
+        <v>24350</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -9591,10 +9595,10 @@
         <v>563322</v>
       </c>
       <c r="F15" s="3">
-        <v>31446</v>
+        <v>23711</v>
       </c>
       <c r="G15" s="3">
-        <v>48448</v>
+        <v>36165</v>
       </c>
       <c r="H15" s="3">
         <v>26137</v>
@@ -9603,10 +9607,10 @@
         <v>41396</v>
       </c>
       <c r="J15" s="3">
-        <v>57583</v>
+        <v>49848</v>
       </c>
       <c r="K15" s="3">
-        <v>734167</v>
+        <v>721884</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -9622,10 +9626,10 @@
         <v>141763</v>
       </c>
       <c r="F16" s="3">
-        <v>9549</v>
+        <v>7274</v>
       </c>
       <c r="G16" s="3">
-        <v>15803</v>
+        <v>10745</v>
       </c>
       <c r="H16" s="3">
         <v>7537</v>
@@ -9634,10 +9638,10 @@
         <v>12818</v>
       </c>
       <c r="J16" s="3">
-        <v>17086</v>
+        <v>14811</v>
       </c>
       <c r="K16" s="3">
-        <v>188283</v>
+        <v>183225</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -9653,10 +9657,10 @@
         <v>2691804</v>
       </c>
       <c r="F17" s="3">
-        <v>163275</v>
+        <v>153265</v>
       </c>
       <c r="G17" s="3">
-        <v>251380</v>
+        <v>233941</v>
       </c>
       <c r="H17" s="3">
         <v>169549</v>
@@ -9665,10 +9669,10 @@
         <v>275473</v>
       </c>
       <c r="J17" s="3">
-        <v>332824</v>
+        <v>322814</v>
       </c>
       <c r="K17" s="3">
-        <v>3634384</v>
+        <v>3616945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>